<commit_message>
Figure S3 & Table S8
</commit_message>
<xml_diff>
--- a/benchmarks/summary_S01.xlsx
+++ b/benchmarks/summary_S01.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="summary_suppl_table" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="summary_suppl_table_S7" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="summary_suppl_table_S8" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="70">
   <si>
     <t xml:space="preserve">Metrics type</t>
   </si>
@@ -156,6 +157,12 @@
   </si>
   <si>
     <t xml:space="preserve">-***</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S01AliCMclean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S01AliCM</t>
   </si>
   <si>
     <r>
@@ -273,6 +280,30 @@
   </si>
   <si>
     <t xml:space="preserve">alignment + shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-*</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We used ShapeSorter web-server and thus couldn’t measure the running time</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -675,10 +706,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ42"/>
+  <dimension ref="A1:AMJ57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F38" activeCellId="0" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2281,84 +2312,699 @@
         <v>134.1</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="36" t="s">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
-      <c r="K38" s="36"/>
-      <c r="L38" s="36"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="37" t="s">
+      <c r="B38" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="18" t="n">
+        <f aca="false">ROUND(2*F38*I38/(F38+I38),3)</f>
+        <v>0.664</v>
+      </c>
+      <c r="D38" s="18" t="n">
+        <f aca="false">ROUND(2*G38*J38/(G38+J38),3)</f>
+        <v>0.874</v>
+      </c>
+      <c r="E38" s="19" t="n">
+        <f aca="false">ROUND(2*H38*K38/(H38+K38),3)</f>
+        <v>0.557</v>
+      </c>
+      <c r="F38" s="20" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="G38" s="20" t="n">
+        <v>0.868</v>
+      </c>
+      <c r="H38" s="20" t="n">
+        <v>0.544</v>
+      </c>
+      <c r="I38" s="21" t="n">
+        <v>0.661</v>
+      </c>
+      <c r="J38" s="20" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K38" s="22" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="L38" s="22" t="n">
+        <v>419.9</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="25" t="n">
+        <f aca="false">ROUND(2*F39*I39/(F39+I39),3)</f>
+        <v>0.63</v>
+      </c>
+      <c r="D39" s="25" t="n">
+        <f aca="false">ROUND(2*G39*J39/(G39+J39),3)</f>
+        <v>0.775</v>
+      </c>
+      <c r="E39" s="26" t="n">
+        <f aca="false">ROUND(2*H39*K39/(H39+K39),3)</f>
+        <v>0.554</v>
+      </c>
+      <c r="F39" s="23" t="n">
+        <v>0.632</v>
+      </c>
+      <c r="G39" s="23" t="n">
+        <v>0.748</v>
+      </c>
+      <c r="H39" s="23" t="n">
+        <v>0.547</v>
+      </c>
+      <c r="I39" s="27" t="n">
+        <v>0.629</v>
+      </c>
+      <c r="J39" s="23" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="K39" s="28" t="n">
+        <v>0.562</v>
+      </c>
+      <c r="L39" s="28" t="n">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="25" t="n">
+        <f aca="false">ROUND(2*F40*I40/(F40+I40),3)</f>
+        <v>0.743</v>
+      </c>
+      <c r="D40" s="25" t="n">
+        <f aca="false">ROUND(2*G40*J40/(G40+J40),3)</f>
+        <v>0.863</v>
+      </c>
+      <c r="E40" s="26" t="n">
+        <f aca="false">ROUND(2*H40*K40/(H40+K40),3)</f>
+        <v>0.661</v>
+      </c>
+      <c r="F40" s="35" t="n">
+        <v>0.729</v>
+      </c>
+      <c r="G40" s="35" t="n">
+        <v>0.839</v>
+      </c>
+      <c r="H40" s="35" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="I40" s="27" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="J40" s="23" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="K40" s="28" t="n">
+        <v>0.679</v>
+      </c>
+      <c r="L40" s="28" t="n">
+        <v>353.8</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="25" t="n">
+        <f aca="false">ROUND(2*F41*I41/(F41+I41),3)</f>
+        <v>0.656</v>
+      </c>
+      <c r="D41" s="25" t="n">
+        <f aca="false">ROUND(2*G41*J41/(G41+J41),3)</f>
+        <v>0.725</v>
+      </c>
+      <c r="E41" s="26" t="n">
+        <f aca="false">ROUND(2*H41*K41/(H41+K41),3)</f>
+        <v>0.604</v>
+      </c>
+      <c r="F41" s="35" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G41" s="35" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H41" s="35" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="I41" s="27" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="J41" s="23" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="K41" s="28" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="L41" s="28" t="n">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="25" t="n">
+        <f aca="false">ROUND(2*F42*I42/(F42+I42),3)</f>
+        <v>0.656</v>
+      </c>
+      <c r="D42" s="25" t="n">
+        <f aca="false">ROUND(2*G42*J42/(G42+J42),3)</f>
+        <v>0.725</v>
+      </c>
+      <c r="E42" s="26" t="n">
+        <f aca="false">ROUND(2*H42*K42/(H42+K42),3)</f>
+        <v>0.604</v>
+      </c>
+      <c r="F42" s="35" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G42" s="35" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H42" s="35" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="I42" s="27" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="J42" s="23" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="K42" s="28" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="L42" s="28" t="n">
+        <v>153.8</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="25" t="n">
+        <f aca="false">ROUND(2*F43*I43/(F43+I43),3)</f>
+        <v>0.585</v>
+      </c>
+      <c r="D43" s="25" t="n">
+        <f aca="false">ROUND(2*G43*J43/(G43+J43),3)</f>
+        <v>0.672</v>
+      </c>
+      <c r="E43" s="26" t="n">
+        <f aca="false">ROUND(2*H43*K43/(H43+K43),3)</f>
+        <v>0.527</v>
+      </c>
+      <c r="F43" s="23" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="G43" s="23" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="H43" s="23" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="I43" s="27" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="J43" s="23" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="K43" s="28" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="L43" s="28" t="n">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C44" s="25" t="n">
+        <f aca="false">ROUND(2*F44*I44/(F44+I44),3)</f>
+        <v>0.629</v>
+      </c>
+      <c r="D44" s="25" t="n">
+        <f aca="false">ROUND(2*G44*J44/(G44+J44),3)</f>
+        <v>0.637</v>
+      </c>
+      <c r="E44" s="26" t="n">
+        <f aca="false">ROUND(2*H44*K44/(H44+K44),3)</f>
+        <v>0.626</v>
+      </c>
+      <c r="F44" s="23" t="n">
+        <v>0.592</v>
+      </c>
+      <c r="G44" s="23" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="H44" s="23" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="I44" s="27" t="n">
+        <v>0.672</v>
+      </c>
+      <c r="J44" s="23" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="K44" s="28" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="L44" s="28" t="n">
+        <v>230.2</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="25" t="n">
+        <f aca="false">ROUND(2*F45*I45/(F45+I45),3)</f>
+        <v>0.605</v>
+      </c>
+      <c r="D45" s="25" t="n">
+        <f aca="false">ROUND(2*G45*J45/(G45+J45),3)</f>
+        <v>0.807</v>
+      </c>
+      <c r="E45" s="26" t="n">
+        <f aca="false">ROUND(2*H45*K45/(H45+K45),3)</f>
+        <v>0.505</v>
+      </c>
+      <c r="F45" s="23" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G45" s="23" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="H45" s="23" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="I45" s="27" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="J45" s="23" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="K45" s="28" t="n">
+        <v>0.578</v>
+      </c>
+      <c r="L45" s="28" t="n">
+        <v>228.4</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C46" s="29" t="n">
+        <f aca="false">ROUND(2*F46*I46/(F46+I46),3)</f>
+        <v>0.611</v>
+      </c>
+      <c r="D46" s="29" t="n">
+        <f aca="false">ROUND(2*G46*J46/(G46+J46),3)</f>
+        <v>0.613</v>
+      </c>
+      <c r="E46" s="30" t="n">
+        <f aca="false">ROUND(2*H46*K46/(H46+K46),3)</f>
+        <v>0.612</v>
+      </c>
+      <c r="F46" s="31" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="G46" s="31" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H46" s="31" t="n">
+        <v>0.563</v>
+      </c>
+      <c r="I46" s="32" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="J46" s="31" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="K46" s="33" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="L46" s="33" t="n">
+        <v>228.1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="37"/>
-      <c r="D39" s="37"/>
-      <c r="E39" s="37"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="37"/>
-      <c r="H39" s="37"/>
-      <c r="I39" s="37"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="37"/>
-      <c r="L39" s="37"/>
-    </row>
-    <row r="40" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="37"/>
-      <c r="B40" s="37"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="37"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
-      <c r="K40" s="37"/>
-      <c r="L40" s="37"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="38" t="s">
+      <c r="B47" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="25" t="n">
+        <f aca="false">ROUND(2*F47*I47/(F47+I47),3)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D47" s="25" t="n">
+        <f aca="false">ROUND(2*G47*J47/(G47+J47),3)</f>
+        <v>0.734</v>
+      </c>
+      <c r="E47" s="26" t="n">
+        <f aca="false">ROUND(2*H47*K47/(H47+K47),3)</f>
+        <v>0.524</v>
+      </c>
+      <c r="F47" s="23" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="G47" s="23" t="n">
+        <v>0.719</v>
+      </c>
+      <c r="H47" s="23" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="I47" s="27" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="J47" s="23" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K47" s="28" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L47" s="28" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="25" t="n">
+        <f aca="false">ROUND(2*F48*I48/(F48+I48),3)</f>
+        <v>0.344</v>
+      </c>
+      <c r="D48" s="25" t="n">
+        <f aca="false">ROUND(2*G48*J48/(G48+J48),3)</f>
+        <v>0.891</v>
+      </c>
+      <c r="E48" s="26" t="n">
+        <f aca="false">ROUND(2*H48*K48/(H48+K48),3)</f>
+        <v>0.231</v>
+      </c>
+      <c r="F48" s="23" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G48" s="23" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="H48" s="23" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="I48" s="27" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="J48" s="23" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="K48" s="28" t="n">
+        <v>0.234</v>
+      </c>
+      <c r="L48" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="25" t="n">
+        <f aca="false">ROUND(2*F49*I49/(F49+I49),3)</f>
+        <v>0.64</v>
+      </c>
+      <c r="D49" s="25" t="n">
+        <f aca="false">ROUND(2*G49*J49/(G49+J49),3)</f>
+        <v>0.694</v>
+      </c>
+      <c r="E49" s="26" t="n">
+        <f aca="false">ROUND(2*H49*K49/(H49+K49),3)</f>
+        <v>0.597</v>
+      </c>
+      <c r="F49" s="23" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="G49" s="23" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="H49" s="23" t="n">
+        <v>0.547</v>
+      </c>
+      <c r="I49" s="27" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="J49" s="23" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="K49" s="28" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="L49" s="28" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" s="25" t="n">
+        <f aca="false">ROUND(2*F50*I50/(F50+I50),3)</f>
+        <v>0.681</v>
+      </c>
+      <c r="D50" s="25" t="n">
+        <f aca="false">ROUND(2*G50*J50/(G50+J50),3)</f>
+        <v>0.676</v>
+      </c>
+      <c r="E50" s="26" t="n">
+        <f aca="false">ROUND(2*H50*K50/(H50+K50),3)</f>
+        <v>0.69</v>
+      </c>
+      <c r="F50" s="23" t="n">
+        <v>0.651</v>
+      </c>
+      <c r="G50" s="23" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="H50" s="23" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="I50" s="27" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="J50" s="23" t="n">
+        <v>0.702</v>
+      </c>
+      <c r="K50" s="28" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="L50" s="28" t="n">
+        <v>248.7</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="25" t="n">
+        <f aca="false">ROUND(2*F51*I51/(F51+I51),3)</f>
+        <v>0.676</v>
+      </c>
+      <c r="D51" s="25" t="n">
+        <f aca="false">ROUND(2*G51*J51/(G51+J51),3)</f>
+        <v>0.832</v>
+      </c>
+      <c r="E51" s="26" t="n">
+        <f aca="false">ROUND(2*H51*K51/(H51+K51),3)</f>
+        <v>0.58</v>
+      </c>
+      <c r="F51" s="23" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="G51" s="23" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="H51" s="23" t="n">
+        <v>0.529</v>
+      </c>
+      <c r="I51" s="27" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="J51" s="23" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="K51" s="28" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="L51" s="28" t="n">
+        <v>245.4</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="29" t="n">
+        <f aca="false">ROUND(2*F52*I52/(F52+I52),3)</f>
+        <v>0.644</v>
+      </c>
+      <c r="D52" s="29" t="n">
+        <f aca="false">ROUND(2*G52*J52/(G52+J52),3)</f>
+        <v>0.635</v>
+      </c>
+      <c r="E52" s="30" t="n">
+        <f aca="false">ROUND(2*H52*K52/(H52+K52),3)</f>
+        <v>0.658</v>
+      </c>
+      <c r="F52" s="31" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G52" s="31" t="n">
+        <v>0.606</v>
+      </c>
+      <c r="H52" s="31" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="I52" s="32" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="J52" s="31" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="K52" s="33" t="n">
+        <v>0.708</v>
+      </c>
+      <c r="L52" s="33" t="n">
+        <v>246.3</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="38"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="38"/>
-      <c r="E41" s="38"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
-      <c r="J41" s="38"/>
-      <c r="K41" s="38"/>
-      <c r="L41" s="38"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="38"/>
-      <c r="B42" s="38"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="38"/>
-      <c r="F42" s="38"/>
-      <c r="G42" s="38"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="36"/>
+      <c r="L53" s="36"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="37"/>
+      <c r="J54" s="37"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+    </row>
+    <row r="55" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="37"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="37"/>
+      <c r="J55" s="37"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B56" s="38"/>
+      <c r="C56" s="38"/>
+      <c r="D56" s="38"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="38"/>
+      <c r="G56" s="38"/>
+      <c r="H56" s="38"/>
+      <c r="I56" s="38"/>
+      <c r="J56" s="38"/>
+      <c r="K56" s="38"/>
+      <c r="L56" s="38"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="38"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="38"/>
+      <c r="E57" s="38"/>
+      <c r="F57" s="38"/>
+      <c r="G57" s="38"/>
+      <c r="H57" s="38"/>
+      <c r="I57" s="38"/>
+      <c r="J57" s="38"/>
+      <c r="K57" s="38"/>
+      <c r="L57" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
+  <mergeCells count="24">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
@@ -2378,9 +3024,11 @@
     <mergeCell ref="A15:A22"/>
     <mergeCell ref="A23:A31"/>
     <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="A39:L40"/>
-    <mergeCell ref="A41:L42"/>
+    <mergeCell ref="A38:A46"/>
+    <mergeCell ref="A47:A52"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A54:L55"/>
+    <mergeCell ref="A56:L57"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2399,7 +3047,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O12" activeCellId="0" sqref="O12"/>
     </sheetView>
   </sheetViews>
@@ -2493,7 +3141,7 @@
     </row>
     <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="40" t="s">
         <v>10</v>
@@ -2519,7 +3167,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="39" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="40" t="s">
         <v>12</v>
@@ -2566,7 +3214,7 @@
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39"/>
       <c r="B5" s="40" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" s="41" t="n">
         <f aca="false">ROUND(2*F5*I5/(F5+I5),3)</f>
@@ -2658,7 +3306,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C7" s="41" t="n">
         <f aca="false">ROUND(2*F7*I7/(F7+I7),3)</f>
@@ -2702,7 +3350,7 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="39"/>
       <c r="B8" s="40" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C8" s="43" t="n">
         <f aca="false">ROUND(2*F8*I8/(F8+I8),3)</f>
@@ -2840,7 +3488,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C11" s="41" t="n">
         <f aca="false">ROUND(2*F11*I11/(F11+I11),3)</f>
@@ -2886,7 +3534,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C12" s="41" t="n">
         <f aca="false">ROUND(2*F12*I12/(F12+I12),3)</f>
@@ -2932,7 +3580,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C13" s="41" t="n">
         <f aca="false">ROUND(2*F13*I13/(F13+I13),3)</f>
@@ -2978,7 +3626,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C14" s="41" t="n">
         <f aca="false">ROUND(2*F14*I14/(F14+I14),3)</f>
@@ -3021,7 +3669,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="39" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B15" s="40" t="s">
         <v>12</v>
@@ -3068,7 +3716,7 @@
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="39"/>
       <c r="B16" s="40" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" s="41" t="n">
         <f aca="false">ROUND(2*F16*I16/(F16+I16),3)</f>
@@ -3114,7 +3762,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="41" t="n">
         <f aca="false">ROUND(2*F17*I17/(F17+I17),3)</f>
@@ -3158,7 +3806,7 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="39"/>
       <c r="B18" s="40" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C18" s="43" t="n">
         <f aca="false">ROUND(2*F18*I18/(F18+I18),3)</f>
@@ -3204,7 +3852,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C19" s="41" t="n">
         <f aca="false">ROUND(2*F19*I19/(F19+I19),3)</f>
@@ -3250,7 +3898,7 @@
         <v>28</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C20" s="41" t="n">
         <f aca="false">ROUND(2*F20*I20/(F20+I20),3)</f>
@@ -3296,7 +3944,7 @@
         <v>28</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C21" s="41" t="n">
         <f aca="false">ROUND(2*F21*I21/(F21+I21),3)</f>
@@ -3342,7 +3990,7 @@
         <v>28</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C22" s="41" t="n">
         <f aca="false">ROUND(2*F22*I22/(F22+I22),3)</f>
@@ -3385,7 +4033,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="39" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B23" s="40" t="s">
         <v>34</v>
@@ -3516,7 +4164,7 @@
         <v>33</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C26" s="41" t="n">
         <f aca="false">ROUND(2*F26*I26/(F26+I26),3)</f>
@@ -3557,7 +4205,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C27" s="41" t="n">
         <f aca="false">ROUND(2*F27*I27/(F27+I27),3)</f>
@@ -3598,7 +4246,7 @@
         <v>33</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C28" s="41" t="n">
         <f aca="false">ROUND(2*F28*I28/(F28+I28),3)</f>
@@ -3639,7 +4287,7 @@
         <v>33</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C29" s="41" t="n">
         <f aca="false">ROUND(2*F29*I29/(F29+I29),3)</f>
@@ -3680,7 +4328,7 @@
         <v>33</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C30" s="41" t="n">
         <f aca="false">ROUND(2*F30*I30/(F30+I30),3)</f>
@@ -3721,7 +4369,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C31" s="41" t="n">
         <f aca="false">ROUND(2*F31*I31/(F31+I31),3)</f>
@@ -3759,7 +4407,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="39" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B32" s="40" t="s">
         <v>35</v>
@@ -3844,7 +4492,7 @@
         <v>42</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C34" s="41" t="n">
         <f aca="false">ROUND(2*F34*I34/(F34+I34),3)</f>
@@ -3885,7 +4533,7 @@
         <v>42</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C35" s="43" t="n">
         <f aca="false">ROUND(2*F35*I35/(F35+I35),3)</f>
@@ -3926,7 +4574,7 @@
         <v>42</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C36" s="41" t="n">
         <f aca="false">ROUND(2*F36*I36/(F36+I36),3)</f>
@@ -3967,7 +4615,7 @@
         <v>42</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C37" s="41" t="n">
         <f aca="false">ROUND(2*F37*I37/(F37+I37),3)</f>
@@ -4005,7 +4653,7 @@
     </row>
     <row r="38" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="47" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B38" s="47"/>
       <c r="C38" s="47"/>
@@ -4021,7 +4669,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B39" s="47"/>
       <c r="C39" s="47"/>
@@ -4051,7 +4699,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B41" s="48"/>
       <c r="C41" s="48"/>
@@ -4112,4 +4760,810 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O35" activeCellId="0" sqref="O35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="19.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="3" style="3" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="3" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="11.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="15.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="18" style="3" width="11.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1022" style="5" width="11.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="AMH1" s="11"/>
+      <c r="AMI1" s="11"/>
+      <c r="AMJ1" s="11"/>
+    </row>
+    <row r="2" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="39"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
+      <c r="P2" s="10"/>
+      <c r="Q2" s="10"/>
+      <c r="AMH2" s="11"/>
+      <c r="AMI2" s="11"/>
+      <c r="AMJ2" s="11"/>
+    </row>
+    <row r="3" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="AMH3" s="11"/>
+      <c r="AMI3" s="11"/>
+      <c r="AMJ3" s="11"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="41" t="n">
+        <f aca="false">ROUND(2*F4*I4/(F4+I4),3)</f>
+        <v>0.664</v>
+      </c>
+      <c r="D4" s="43" t="n">
+        <f aca="false">ROUND(2*G4*J4/(G4+J4),3)</f>
+        <v>0.874</v>
+      </c>
+      <c r="E4" s="41" t="n">
+        <f aca="false">ROUND(2*H4*K4/(H4+K4),3)</f>
+        <v>0.557</v>
+      </c>
+      <c r="F4" s="42" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="G4" s="44" t="n">
+        <v>0.868</v>
+      </c>
+      <c r="H4" s="42" t="n">
+        <v>0.544</v>
+      </c>
+      <c r="I4" s="42" t="n">
+        <v>0.661</v>
+      </c>
+      <c r="J4" s="42" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K4" s="42" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="L4" s="42" t="n">
+        <v>419.9</v>
+      </c>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="41" t="n">
+        <f aca="false">ROUND(2*F5*I5/(F5+I5),3)</f>
+        <v>0.63</v>
+      </c>
+      <c r="D5" s="41" t="n">
+        <f aca="false">ROUND(2*G5*J5/(G5+J5),3)</f>
+        <v>0.775</v>
+      </c>
+      <c r="E5" s="41" t="n">
+        <f aca="false">ROUND(2*H5*K5/(H5+K5),3)</f>
+        <v>0.554</v>
+      </c>
+      <c r="F5" s="42" t="n">
+        <v>0.632</v>
+      </c>
+      <c r="G5" s="42" t="n">
+        <v>0.748</v>
+      </c>
+      <c r="H5" s="42" t="n">
+        <v>0.547</v>
+      </c>
+      <c r="I5" s="42" t="n">
+        <v>0.629</v>
+      </c>
+      <c r="J5" s="42" t="n">
+        <v>0.805</v>
+      </c>
+      <c r="K5" s="42" t="n">
+        <v>0.562</v>
+      </c>
+      <c r="L5" s="42" t="n">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="43" t="n">
+        <f aca="false">ROUND(2*F6*I6/(F6+I6),3)</f>
+        <v>0.743</v>
+      </c>
+      <c r="D6" s="41" t="n">
+        <f aca="false">ROUND(2*G6*J6/(G6+J6),3)</f>
+        <v>0.863</v>
+      </c>
+      <c r="E6" s="43" t="n">
+        <f aca="false">ROUND(2*H6*K6/(H6+K6),3)</f>
+        <v>0.661</v>
+      </c>
+      <c r="F6" s="45" t="n">
+        <v>0.729</v>
+      </c>
+      <c r="G6" s="46" t="n">
+        <v>0.839</v>
+      </c>
+      <c r="H6" s="45" t="n">
+        <v>0.644</v>
+      </c>
+      <c r="I6" s="44" t="n">
+        <v>0.757</v>
+      </c>
+      <c r="J6" s="44" t="n">
+        <v>0.889</v>
+      </c>
+      <c r="K6" s="42" t="n">
+        <v>0.679</v>
+      </c>
+      <c r="L6" s="42" t="n">
+        <v>353.8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="41" t="n">
+        <f aca="false">ROUND(2*F7*I7/(F7+I7),3)</f>
+        <v>0.656</v>
+      </c>
+      <c r="D7" s="41" t="n">
+        <f aca="false">ROUND(2*G7*J7/(G7+J7),3)</f>
+        <v>0.725</v>
+      </c>
+      <c r="E7" s="41" t="n">
+        <f aca="false">ROUND(2*H7*K7/(H7+K7),3)</f>
+        <v>0.604</v>
+      </c>
+      <c r="F7" s="46" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G7" s="46" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H7" s="46" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="I7" s="42" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="J7" s="42" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="K7" s="42" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="L7" s="42" t="n">
+        <v>152.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="41" t="n">
+        <f aca="false">ROUND(2*F8*I8/(F8+I8),3)</f>
+        <v>0.656</v>
+      </c>
+      <c r="D8" s="41" t="n">
+        <f aca="false">ROUND(2*G8*J8/(G8+J8),3)</f>
+        <v>0.725</v>
+      </c>
+      <c r="E8" s="41" t="n">
+        <f aca="false">ROUND(2*H8*K8/(H8+K8),3)</f>
+        <v>0.604</v>
+      </c>
+      <c r="F8" s="46" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="G8" s="46" t="n">
+        <v>0.698</v>
+      </c>
+      <c r="H8" s="46" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="I8" s="42" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="J8" s="42" t="n">
+        <v>0.755</v>
+      </c>
+      <c r="K8" s="42" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="L8" s="42" t="n">
+        <v>153.8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="41" t="n">
+        <f aca="false">ROUND(2*F9*I9/(F9+I9),3)</f>
+        <v>0.585</v>
+      </c>
+      <c r="D9" s="41" t="n">
+        <f aca="false">ROUND(2*G9*J9/(G9+J9),3)</f>
+        <v>0.672</v>
+      </c>
+      <c r="E9" s="41" t="n">
+        <f aca="false">ROUND(2*H9*K9/(H9+K9),3)</f>
+        <v>0.527</v>
+      </c>
+      <c r="F9" s="42" t="n">
+        <v>0.543</v>
+      </c>
+      <c r="G9" s="42" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="H9" s="42" t="n">
+        <v>0.472</v>
+      </c>
+      <c r="I9" s="42" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="J9" s="42" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="K9" s="42" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="L9" s="42" t="n">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="41" t="n">
+        <f aca="false">ROUND(2*F10*I10/(F10+I10),3)</f>
+        <v>0.629</v>
+      </c>
+      <c r="D10" s="41" t="n">
+        <f aca="false">ROUND(2*G10*J10/(G10+J10),3)</f>
+        <v>0.637</v>
+      </c>
+      <c r="E10" s="41" t="n">
+        <f aca="false">ROUND(2*H10*K10/(H10+K10),3)</f>
+        <v>0.626</v>
+      </c>
+      <c r="F10" s="42" t="n">
+        <v>0.592</v>
+      </c>
+      <c r="G10" s="42" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="H10" s="42" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="I10" s="42" t="n">
+        <v>0.672</v>
+      </c>
+      <c r="J10" s="42" t="n">
+        <v>0.673</v>
+      </c>
+      <c r="K10" s="44" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="L10" s="42" t="n">
+        <v>230.2</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="41" t="n">
+        <f aca="false">ROUND(2*F11*I11/(F11+I11),3)</f>
+        <v>0.605</v>
+      </c>
+      <c r="D11" s="41" t="n">
+        <f aca="false">ROUND(2*G11*J11/(G11+J11),3)</f>
+        <v>0.807</v>
+      </c>
+      <c r="E11" s="41" t="n">
+        <f aca="false">ROUND(2*H11*K11/(H11+K11),3)</f>
+        <v>0.505</v>
+      </c>
+      <c r="F11" s="42" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="G11" s="42" t="n">
+        <v>0.785</v>
+      </c>
+      <c r="H11" s="42" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="I11" s="42" t="n">
+        <v>0.645</v>
+      </c>
+      <c r="J11" s="42" t="n">
+        <v>0.83</v>
+      </c>
+      <c r="K11" s="42" t="n">
+        <v>0.578</v>
+      </c>
+      <c r="L11" s="42" t="n">
+        <v>228.4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="41" t="n">
+        <f aca="false">ROUND(2*F12*I12/(F12+I12),3)</f>
+        <v>0.611</v>
+      </c>
+      <c r="D12" s="41" t="n">
+        <f aca="false">ROUND(2*G12*J12/(G12+J12),3)</f>
+        <v>0.613</v>
+      </c>
+      <c r="E12" s="41" t="n">
+        <f aca="false">ROUND(2*H12*K12/(H12+K12),3)</f>
+        <v>0.612</v>
+      </c>
+      <c r="F12" s="42" t="n">
+        <v>0.569</v>
+      </c>
+      <c r="G12" s="42" t="n">
+        <v>0.576</v>
+      </c>
+      <c r="H12" s="42" t="n">
+        <v>0.563</v>
+      </c>
+      <c r="I12" s="42" t="n">
+        <v>0.659</v>
+      </c>
+      <c r="J12" s="42" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="K12" s="42" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="L12" s="42" t="n">
+        <v>228.1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="41" t="n">
+        <f aca="false">ROUND(2*F13*I13/(F13+I13),3)</f>
+        <v>0.6</v>
+      </c>
+      <c r="D13" s="41" t="n">
+        <f aca="false">ROUND(2*G13*J13/(G13+J13),3)</f>
+        <v>0.734</v>
+      </c>
+      <c r="E13" s="41" t="n">
+        <f aca="false">ROUND(2*H13*K13/(H13+K13),3)</f>
+        <v>0.524</v>
+      </c>
+      <c r="F13" s="42" t="n">
+        <v>0.605</v>
+      </c>
+      <c r="G13" s="42" t="n">
+        <v>0.719</v>
+      </c>
+      <c r="H13" s="42" t="n">
+        <v>0.522</v>
+      </c>
+      <c r="I13" s="42" t="n">
+        <v>0.595</v>
+      </c>
+      <c r="J13" s="42" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="K13" s="42" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L13" s="42" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="41" t="n">
+        <f aca="false">ROUND(2*F14*I14/(F14+I14),3)</f>
+        <v>0.344</v>
+      </c>
+      <c r="D14" s="43" t="n">
+        <f aca="false">ROUND(2*G14*J14/(G14+J14),3)</f>
+        <v>0.891</v>
+      </c>
+      <c r="E14" s="41" t="n">
+        <f aca="false">ROUND(2*H14*K14/(H14+K14),3)</f>
+        <v>0.231</v>
+      </c>
+      <c r="F14" s="42" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="G14" s="44" t="n">
+        <v>0.855</v>
+      </c>
+      <c r="H14" s="42" t="n">
+        <v>0.228</v>
+      </c>
+      <c r="I14" s="42" t="n">
+        <v>0.329</v>
+      </c>
+      <c r="J14" s="44" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="K14" s="42" t="n">
+        <v>0.234</v>
+      </c>
+      <c r="L14" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="41" t="n">
+        <f aca="false">ROUND(2*F15*I15/(F15+I15),3)</f>
+        <v>0.64</v>
+      </c>
+      <c r="D15" s="41" t="n">
+        <f aca="false">ROUND(2*G15*J15/(G15+J15),3)</f>
+        <v>0.694</v>
+      </c>
+      <c r="E15" s="41" t="n">
+        <f aca="false">ROUND(2*H15*K15/(H15+K15),3)</f>
+        <v>0.597</v>
+      </c>
+      <c r="F15" s="42" t="n">
+        <v>0.602</v>
+      </c>
+      <c r="G15" s="42" t="n">
+        <v>0.669</v>
+      </c>
+      <c r="H15" s="42" t="n">
+        <v>0.547</v>
+      </c>
+      <c r="I15" s="42" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="J15" s="42" t="n">
+        <v>0.722</v>
+      </c>
+      <c r="K15" s="42" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="L15" s="42" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="43" t="n">
+        <f aca="false">ROUND(2*F16*I16/(F16+I16),3)</f>
+        <v>0.681</v>
+      </c>
+      <c r="D16" s="41" t="n">
+        <f aca="false">ROUND(2*G16*J16/(G16+J16),3)</f>
+        <v>0.676</v>
+      </c>
+      <c r="E16" s="43" t="n">
+        <f aca="false">ROUND(2*H16*K16/(H16+K16),3)</f>
+        <v>0.69</v>
+      </c>
+      <c r="F16" s="44" t="n">
+        <v>0.651</v>
+      </c>
+      <c r="G16" s="42" t="n">
+        <v>0.652</v>
+      </c>
+      <c r="H16" s="44" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="I16" s="44" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="J16" s="42" t="n">
+        <v>0.702</v>
+      </c>
+      <c r="K16" s="44" t="n">
+        <v>0.736</v>
+      </c>
+      <c r="L16" s="42" t="n">
+        <v>248.7</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="41" t="n">
+        <f aca="false">ROUND(2*F17*I17/(F17+I17),3)</f>
+        <v>0.676</v>
+      </c>
+      <c r="D17" s="41" t="n">
+        <f aca="false">ROUND(2*G17*J17/(G17+J17),3)</f>
+        <v>0.832</v>
+      </c>
+      <c r="E17" s="41" t="n">
+        <f aca="false">ROUND(2*H17*K17/(H17+K17),3)</f>
+        <v>0.58</v>
+      </c>
+      <c r="F17" s="42" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="G17" s="42" t="n">
+        <v>0.819</v>
+      </c>
+      <c r="H17" s="42" t="n">
+        <v>0.529</v>
+      </c>
+      <c r="I17" s="44" t="n">
+        <v>0.713</v>
+      </c>
+      <c r="J17" s="42" t="n">
+        <v>0.846</v>
+      </c>
+      <c r="K17" s="42" t="n">
+        <v>0.643</v>
+      </c>
+      <c r="L17" s="42" t="n">
+        <v>245.4</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="41" t="n">
+        <f aca="false">ROUND(2*F18*I18/(F18+I18),3)</f>
+        <v>0.644</v>
+      </c>
+      <c r="D18" s="41" t="n">
+        <f aca="false">ROUND(2*G18*J18/(G18+J18),3)</f>
+        <v>0.635</v>
+      </c>
+      <c r="E18" s="41" t="n">
+        <f aca="false">ROUND(2*H18*K18/(H18+K18),3)</f>
+        <v>0.658</v>
+      </c>
+      <c r="F18" s="42" t="n">
+        <v>0.61</v>
+      </c>
+      <c r="G18" s="42" t="n">
+        <v>0.606</v>
+      </c>
+      <c r="H18" s="42" t="n">
+        <v>0.615</v>
+      </c>
+      <c r="I18" s="42" t="n">
+        <v>0.683</v>
+      </c>
+      <c r="J18" s="42" t="n">
+        <v>0.668</v>
+      </c>
+      <c r="K18" s="42" t="n">
+        <v>0.708</v>
+      </c>
+      <c r="L18" s="42" t="n">
+        <v>246.3</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="48"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="48"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="48"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:L3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A4:A12"/>
+    <mergeCell ref="A13:A18"/>
+    <mergeCell ref="A19:L20"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>